<commit_message>
fixed connection problem, started debug
</commit_message>
<xml_diff>
--- a/small modle/query/sample query results 1.xlsx
+++ b/small modle/query/sample query results 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmue\Documents\git\30Qs\small modle\query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECB7B15-B7C6-4454-A2EE-167F31805BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9D7542-14D7-4DE3-A738-90710278C956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1393,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V5" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
got people for querying
</commit_message>
<xml_diff>
--- a/small modle/query/sample query results 1.xlsx
+++ b/small modle/query/sample query results 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmue\Documents\git\30Qs\small modle\query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750FE8F6-C7E6-4E8B-8377-678EF37CA8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AACFC1-A57B-41C6-85A0-692D68279998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1569,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>